<commit_message>
added selection of xls sheet_name, fixed PyPi long Description
</commit_message>
<xml_diff>
--- a/example/Login Tests/DataDriven.xlsx
+++ b/example/Login Tests/DataDriven.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\robotframework-datadriver\example\Login Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8600FC02-5885-49FD-9BE8-194CB8ECE45B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A425A17-F196-47DD-A627-04E341761D62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46080" yWindow="-16770" windowWidth="43200" windowHeight="23535"/>
+    <workbookView xWindow="-28500" yWindow="-8190" windowWidth="24435" windowHeight="16935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDriven" sheetId="1" r:id="rId1"/>
+    <sheet name="2nd Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>*** Test Cases ***</t>
   </si>
@@ -71,12 +72,39 @@
   </si>
   <si>
     <t>foo</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,48 +587,48 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -616,7 +644,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -911,14 +939,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1049,4 +1077,136 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271415A9-6699-4C0B-9491-6FAE70C49EF2}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Structure to dynamically loading File Reader Classes!
</commit_message>
<xml_diff>
--- a/example/Login Tests/DataDriven.xlsx
+++ b/example/Login Tests/DataDriven.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\robotframework-datadriver\example\Login Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A425A17-F196-47DD-A627-04E341761D62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F51CF6-F244-498D-83F1-81B5980F3B47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28500" yWindow="-8190" windowWidth="24435" windowHeight="16935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38790" yWindow="-2115" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDriven" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
   <si>
     <t>*** Test Cases ***</t>
   </si>
@@ -72,33 +72,6 @@
   </si>
   <si>
     <t>foo</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1057,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,45 +1087,61 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1160,45 +1149,53 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>